<commit_message>
modified primary key and foreign keys of command table
</commit_message>
<xml_diff>
--- a/Repartition des données.xlsx
+++ b/Repartition des données.xlsx
@@ -191,9 +191,6 @@
     <t xml:space="preserve">pizza</t>
   </si>
   <si>
-    <t xml:space="preserve">pk=user id + pizza id + pizza extra_id + drink id + dessert id + date</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -202,7 +199,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">fk : </t>
+      <t xml:space="preserve">pk=</t>
     </r>
     <r>
       <rPr>
@@ -211,13 +208,8 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">command id, user id, pizza id, productid, productid, productid</t>
+      <t xml:space="preserve">command id + </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">command</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -226,17 +218,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">hash index : command id, </t>
+      <t xml:space="preserve">user id + pizza id + pizza extra_id + drink id + dessert id + date</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">user id, pizza id, pizza extra_id, drink id, dessert id </t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fk : user id, pizza id, productid, productid, productid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hash index : command id, user id, pizza id, pizza extra_id, drink id, dessert id </t>
   </si>
   <si>
     <t xml:space="preserve"> =product id</t>
@@ -656,7 +648,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="14627880" y="5793480"/>
+          <a:off x="14628600" y="5793480"/>
           <a:ext cx="3147120" cy="2239560"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -698,8 +690,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="16072920" y="2853360"/>
-          <a:ext cx="3313080" cy="977760"/>
+          <a:off x="16073640" y="2853360"/>
+          <a:ext cx="3312360" cy="977760"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -782,8 +774,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16288920" y="977040"/>
-          <a:ext cx="3116520" cy="28800"/>
+          <a:off x="16289640" y="977040"/>
+          <a:ext cx="3115800" cy="28800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1370,7 +1362,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.91"/>
@@ -1761,7 +1753,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I19" s="0" t="s">
         <v>56</v>
       </c>
@@ -1781,7 +1773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I20" s="0" t="s">
         <v>57</v>
       </c>

</xml_diff>